<commit_message>
"adding docker basics lab"
</commit_message>
<xml_diff>
--- a/DevOps.xlsx
+++ b/DevOps.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25831"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D3029B6-90C7-483A-B8C4-2E6704A3377B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D57FF995-D70B-4272-A669-D708BBC40796}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DevOps_Basics" sheetId="4" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Terraform" sheetId="2" r:id="rId2"/>
+    <sheet name="docker" sheetId="5" r:id="rId3"/>
+    <sheet name="kubernetes" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="156">
   <si>
     <t>dictionary - should have colon and space before data</t>
   </si>
@@ -413,12 +415,129 @@
   <si>
     <t>dictionaries aew always indicated within curly bracket {}</t>
   </si>
+  <si>
+    <t>what is docker file vs docker compose</t>
+  </si>
+  <si>
+    <t>docker image vs container</t>
+  </si>
+  <si>
+    <t>docker compose</t>
+  </si>
+  <si>
+    <t>what is namespace in docker</t>
+  </si>
+  <si>
+    <t>cgroups</t>
+  </si>
+  <si>
+    <t>docker engine</t>
+  </si>
+  <si>
+    <t>entrypoint in docker file</t>
+  </si>
+  <si>
+    <t>docker storage</t>
+  </si>
+  <si>
+    <t>copy on write</t>
+  </si>
+  <si>
+    <t>volume mount and Bind mount</t>
+  </si>
+  <si>
+    <t>docker networks</t>
+  </si>
+  <si>
+    <t>bridge, none, host</t>
+  </si>
+  <si>
+    <t>user defined networks</t>
+  </si>
+  <si>
+    <t>doubts</t>
+  </si>
+  <si>
+    <t>docker registry</t>
+  </si>
+  <si>
+    <t>docker private registry</t>
+  </si>
+  <si>
+    <t>docker hub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">docker prune </t>
+  </si>
+  <si>
+    <t>topics</t>
+  </si>
+  <si>
+    <t>tasks</t>
+  </si>
+  <si>
+    <t>creating private registry</t>
+  </si>
+  <si>
+    <t>container orchestration</t>
+  </si>
+  <si>
+    <t>docker swarm, kubernetes, mesos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">what happens when you install docker </t>
+  </si>
+  <si>
+    <t>alternaives to docker</t>
+  </si>
+  <si>
+    <t>podman, buildkit, skopio</t>
+  </si>
+  <si>
+    <t>docker commands</t>
+  </si>
+  <si>
+    <t>run, ps, ps -a, images, build, compose up, --links, -p, -d, -e</t>
+  </si>
+  <si>
+    <t>command executed when the container is started</t>
+  </si>
+  <si>
+    <t>default commands run when user doesn’t provide any input</t>
+  </si>
+  <si>
+    <t>https://kodekloud.com/topic/commands-vs-entrypoint/</t>
+  </si>
+  <si>
+    <t>docker daemon, rest api, docker cli will be installed</t>
+  </si>
+  <si>
+    <t>docker file</t>
+  </si>
+  <si>
+    <t>creating image</t>
+  </si>
+  <si>
+    <t>creating networks</t>
+  </si>
+  <si>
+    <t>should it be in sequence ---- docker run --network=wp-mysql-network -e DB_Host=mysql-db -e DB_Password=db_pass123 -p 38080:8080 --name webapp --link mysql-db:mysql-db -d kodekloud/simple-webapp-mysql</t>
+  </si>
+  <si>
+    <t>Isolate containers with a user namespace</t>
+  </si>
+  <si>
+    <t>control groups - limiys the usage of cpu, disk and memory</t>
+  </si>
+  <si>
+    <t>creating containers using docker compose</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -449,8 +568,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -469,6 +601,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -482,12 +620,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -498,6 +635,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -841,7 +986,7 @@
   </sheetPr>
   <dimension ref="A1:B129"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A127" workbookViewId="0">
       <selection activeCell="A61" sqref="A61:A66"/>
     </sheetView>
   </sheetViews>
@@ -852,12 +997,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="4"/>
+      <c r="A2" s="3"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
@@ -879,12 +1024,9 @@
       <c r="A5" t="s">
         <v>95</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
@@ -996,7 +1138,7 @@
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="6" t="s">
         <v>66</v>
       </c>
       <c r="B24" t="s">
@@ -1004,7 +1146,7 @@
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" s="7"/>
+      <c r="A25" s="6"/>
       <c r="B25" t="s">
         <v>64</v>
       </c>
@@ -1058,7 +1200,7 @@
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A35" s="6" t="s">
+      <c r="A35" s="5" t="s">
         <v>103</v>
       </c>
       <c r="B35" t="s">
@@ -1066,49 +1208,49 @@
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A36" s="6"/>
+      <c r="A36" s="5"/>
       <c r="B36" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A37" s="6"/>
+      <c r="A37" s="5"/>
       <c r="B37" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A38" s="6"/>
+      <c r="A38" s="5"/>
       <c r="B38" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A39" s="6"/>
+      <c r="A39" s="5"/>
       <c r="B39" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A40" s="6"/>
+      <c r="A40" s="5"/>
       <c r="B40" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A41" s="6"/>
+      <c r="A41" s="5"/>
       <c r="B41" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A42" s="6"/>
+      <c r="A42" s="5"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A43" s="6"/>
+      <c r="A43" s="5"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A47" s="8" t="s">
+      <c r="A47" s="7" t="s">
         <v>104</v>
       </c>
       <c r="B47" t="s">
@@ -1116,25 +1258,25 @@
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A48" s="8"/>
+      <c r="A48" s="7"/>
       <c r="B48" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A49" s="8"/>
+      <c r="A49" s="7"/>
       <c r="B49" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A50" s="8"/>
+      <c r="A50" s="7"/>
       <c r="B50" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A54" s="6" t="s">
+      <c r="A54" s="5" t="s">
         <v>42</v>
       </c>
       <c r="B54" t="s">
@@ -1142,31 +1284,31 @@
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A55" s="6"/>
+      <c r="A55" s="5"/>
       <c r="B55" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A56" s="6"/>
+      <c r="A56" s="5"/>
       <c r="B56" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A57" s="6"/>
+      <c r="A57" s="5"/>
       <c r="B57" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A58" s="6"/>
+      <c r="A58" s="5"/>
       <c r="B58" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A61" s="6" t="s">
+      <c r="A61" s="5" t="s">
         <v>34</v>
       </c>
       <c r="B61" t="s">
@@ -1174,37 +1316,37 @@
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A62" s="6"/>
+      <c r="A62" s="5"/>
       <c r="B62" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A63" s="6"/>
+      <c r="A63" s="5"/>
       <c r="B63" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A64" s="6"/>
+      <c r="A64" s="5"/>
       <c r="B64" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A65" s="6"/>
+      <c r="A65" s="5"/>
       <c r="B65" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A66" s="6"/>
+      <c r="A66" s="5"/>
       <c r="B66" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A69" s="6" t="s">
+      <c r="A69" s="5" t="s">
         <v>29</v>
       </c>
       <c r="B69" t="s">
@@ -1212,49 +1354,49 @@
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A70" s="6"/>
+      <c r="A70" s="5"/>
       <c r="B70" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A71" s="6"/>
+      <c r="A71" s="5"/>
       <c r="B71" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A72" s="6"/>
+      <c r="A72" s="5"/>
       <c r="B72" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A73" s="6"/>
+      <c r="A73" s="5"/>
       <c r="B73" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A74" s="6"/>
+      <c r="A74" s="5"/>
       <c r="B74" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A75" s="6"/>
+      <c r="A75" s="5"/>
       <c r="B75" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A76" s="6"/>
+      <c r="A76" s="5"/>
       <c r="B76" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A80" s="6" t="s">
+      <c r="A80" s="5" t="s">
         <v>23</v>
       </c>
       <c r="B80" t="s">
@@ -1262,13 +1404,13 @@
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A81" s="6"/>
+      <c r="A81" s="5"/>
       <c r="B81" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A84" s="6" t="s">
+      <c r="A84" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B84" t="s">
@@ -1276,67 +1418,67 @@
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A85" s="6"/>
+      <c r="A85" s="5"/>
       <c r="B85" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A86" s="6"/>
+      <c r="A86" s="5"/>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A87" s="6"/>
+      <c r="A87" s="5"/>
       <c r="B87" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A88" s="6"/>
+      <c r="A88" s="5"/>
       <c r="B88" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A89" s="6"/>
+      <c r="A89" s="5"/>
       <c r="B89" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A90" s="6"/>
+      <c r="A90" s="5"/>
       <c r="B90" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A91" s="6"/>
+      <c r="A91" s="5"/>
       <c r="B91" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A92" s="6"/>
+      <c r="A92" s="5"/>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A93" s="6"/>
+      <c r="A93" s="5"/>
       <c r="B93" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A94" s="6"/>
+      <c r="A94" s="5"/>
       <c r="B94" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A95" s="6"/>
+      <c r="A95" s="5"/>
       <c r="B95" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A99" s="6" t="s">
+      <c r="A99" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B99" t="s">
@@ -1344,49 +1486,49 @@
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A100" s="6"/>
+      <c r="A100" s="5"/>
       <c r="B100" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A101" s="6"/>
+      <c r="A101" s="5"/>
       <c r="B101" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A102" s="6"/>
+      <c r="A102" s="5"/>
       <c r="B102" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A103" s="6"/>
+      <c r="A103" s="5"/>
       <c r="B103" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A104" s="6"/>
+      <c r="A104" s="5"/>
       <c r="B104" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A105" s="6"/>
+      <c r="A105" s="5"/>
       <c r="B105" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A106" s="6"/>
+      <c r="A106" s="5"/>
       <c r="B106" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A109" s="6" t="s">
+      <c r="A109" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B109" t="s">
@@ -1394,43 +1536,43 @@
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A110" s="6"/>
+      <c r="A110" s="5"/>
       <c r="B110" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A111" s="6"/>
+      <c r="A111" s="5"/>
       <c r="B111" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A112" s="6"/>
+      <c r="A112" s="5"/>
       <c r="B112" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A113" s="6"/>
+      <c r="A113" s="5"/>
       <c r="B113" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A114" s="6"/>
+      <c r="A114" s="5"/>
       <c r="B114" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A115" s="6"/>
+      <c r="A115" s="5"/>
       <c r="B115" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A119" s="6" t="s">
+      <c r="A119" s="5" t="s">
         <v>115</v>
       </c>
       <c r="B119" t="s">
@@ -1438,48 +1580,48 @@
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A120" s="6"/>
+      <c r="A120" s="5"/>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A121" s="6"/>
+      <c r="A121" s="5"/>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A122" s="6"/>
+      <c r="A122" s="5"/>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A123" s="6"/>
+      <c r="A123" s="5"/>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A124" s="6"/>
+      <c r="A124" s="5"/>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A125" s="6"/>
+      <c r="A125" s="5"/>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A126" s="6"/>
+      <c r="A126" s="5"/>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A127" s="6"/>
+      <c r="A127" s="5"/>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A128" s="6"/>
+      <c r="A128" s="5"/>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A129" s="6"/>
+      <c r="A129" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A61:A66"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A35:A43"/>
+    <mergeCell ref="A47:A50"/>
+    <mergeCell ref="A54:A58"/>
     <mergeCell ref="A119:A129"/>
     <mergeCell ref="A109:A115"/>
     <mergeCell ref="A80:A81"/>
     <mergeCell ref="A84:A95"/>
     <mergeCell ref="A69:A76"/>
     <mergeCell ref="A99:A106"/>
-    <mergeCell ref="A61:A66"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A35:A43"/>
-    <mergeCell ref="A47:A50"/>
-    <mergeCell ref="A54:A58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1488,6 +1630,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1496,4 +1641,228 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C812C77F-0957-445B-BB4A-DDCABC7FAC56}">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="A1:C40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="33.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="B2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>143</v>
+      </c>
+      <c r="B5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>120</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>121</v>
+      </c>
+      <c r="B8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>123</v>
+      </c>
+      <c r="B9" t="s">
+        <v>145</v>
+      </c>
+      <c r="C9" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>143</v>
+      </c>
+      <c r="B10" t="s">
+        <v>146</v>
+      </c>
+      <c r="C10" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>127</v>
+      </c>
+      <c r="B14" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>138</v>
+      </c>
+      <c r="B20" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>141</v>
+      </c>
+      <c r="B21" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" s="8" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A34" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>137</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1A1984A-2DB4-4092-9E63-7A712B47F7CB}">
+  <sheetPr>
+    <tabColor theme="9" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>